<commit_message>
[ADD] Extended map + new url for connection
</commit_message>
<xml_diff>
--- a/view/map.xlsx
+++ b/view/map.xlsx
@@ -47,8 +47,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0\ _€;\-#,##0\ _€"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -115,12 +116,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -143,11 +148,11 @@
   </sheetPr>
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G36" activeCellId="0" sqref="G36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G47" activeCellId="0" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -825,6 +830,12 @@
       <c r="E34" s="0" t="n">
         <v>160</v>
       </c>
+      <c r="F34" s="0" t="n">
+        <v>159</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>470</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
@@ -839,6 +850,12 @@
       <c r="E35" s="0" t="n">
         <v>200</v>
       </c>
+      <c r="F35" s="0" t="n">
+        <v>214</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>439</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
@@ -853,6 +870,12 @@
       <c r="E36" s="0" t="n">
         <v>240</v>
       </c>
+      <c r="F36" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>441</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
@@ -867,6 +890,12 @@
       <c r="E37" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F37" s="0" t="n">
+        <v>714</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>563</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
@@ -881,6 +910,12 @@
       <c r="E38" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F38" s="0" t="n">
+        <v>657</v>
+      </c>
+      <c r="G38" s="2" t="n">
+        <v>471</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
@@ -895,6 +930,12 @@
       <c r="E39" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F39" s="0" t="n">
+        <v>602</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>407</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
@@ -909,6 +950,12 @@
       <c r="E40" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F40" s="0" t="n">
+        <v>521</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>462</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
@@ -923,6 +970,12 @@
       <c r="E41" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F41" s="0" t="n">
+        <v>462</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>517</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -937,6 +990,12 @@
       <c r="E42" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F42" s="0" t="n">
+        <v>517</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>607</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
@@ -951,6 +1010,12 @@
       <c r="E43" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="F43" s="0" t="n">
+        <v>575</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>611</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
@@ -965,6 +1030,12 @@
       <c r="E44" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="F44" s="0" t="n">
+        <v>659</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>627</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
@@ -979,6 +1050,12 @@
       <c r="E45" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="F45" s="0" t="n">
+        <v>631</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>548</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
@@ -993,6 +1070,12 @@
       <c r="E46" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="F46" s="0" t="n">
+        <v>599</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>503</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
@@ -1006,6 +1089,12 @@
       </c>
       <c r="E47" s="0" t="n">
         <v>100</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>549</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>